<commit_message>
1.complete type check code 2.add test case
</commit_message>
<xml_diff>
--- a/test/excel/Example.xlsx
+++ b/test/excel/Example.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F7F573EC-0637-4F7B-A3F3-ABA4E116843B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{DADAB61B-CFCD-4F2E-A515-9ABA9AEA8E86}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -218,7 +218,7 @@
     <t>{key:int}[]</t>
   </si>
   <si>
-    <t>[{"key":1000},{"key2":100}]</t>
+    <t>[{"key":1000},{"key":100}]</t>
   </si>
 </sst>
 </file>
@@ -604,7 +604,7 @@
   <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
1.remove all test files 2.complete type check 3.add test case
</commit_message>
<xml_diff>
--- a/test/excel/Example.xlsx
+++ b/test/excel/Example.xlsx
@@ -3,56 +3,36 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{DADAB61B-CFCD-4F2E-A515-9ABA9AEA8E86}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{025E7DE6-4628-413D-9A9F-55A38EFA90E2}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
   <si>
     <t>Example</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>第二个单元格是表名:</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>#注释列</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>*int</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>#注释行(key必须是id, 必须在第二行) *开头为类型</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>string</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>字符串类型</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>自定义说明</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>xxxx</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -65,10 +45,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>整型</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>type_short</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -77,10 +53,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>短整型(枚举,布尔)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>type_float</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -89,10 +61,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>浮点型</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>type_double</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -101,18 +69,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>双精度</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>type_int_array</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>定长数组</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>int[2]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -121,10 +81,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>不定长数组</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>[1,2,43,5,6,76,7]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -141,10 +97,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Json格式</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>{"key1":10100,"key2":[100,200]}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -153,61 +105,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>object数组</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>a_array_1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>a_array_2</t>
-  </si>
-  <si>
-    <t>合并数组元素1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>合并数组元素2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>k_dic_1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>v_dic_1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>合并字典格式key1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>合并字典格式value1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>k_dic_2</t>
-  </si>
-  <si>
-    <t>v_dic_2</t>
-  </si>
-  <si>
-    <t>合并字典格式key2</t>
-  </si>
-  <si>
-    <t>合并字典格式value2</t>
-  </si>
-  <si>
-    <t>def</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>atk</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>type_string</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -219,6 +116,88 @@
   </si>
   <si>
     <t>[{"key":1000},{"key":100}]</t>
+  </si>
+  <si>
+    <t>{B1}is csv file name</t>
+  </si>
+  <si>
+    <t>#comment line</t>
+  </si>
+  <si>
+    <t>desc etc…</t>
+  </si>
+  <si>
+    <t># Start With '#' means that this is a comment line</t>
+  </si>
+  <si>
+    <t>string type</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>signed int16</t>
+  </si>
+  <si>
+    <t>float type</t>
+  </si>
+  <si>
+    <t>double type</t>
+  </si>
+  <si>
+    <t>object array with {key:integer} type</t>
+  </si>
+  <si>
+    <t>char_type</t>
+  </si>
+  <si>
+    <t>char</t>
+  </si>
+  <si>
+    <t>in range(-128, 127)
+if empty default value is zero</t>
+  </si>
+  <si>
+    <t>multi_arry</t>
+  </si>
+  <si>
+    <t>int[][2]</t>
+  </si>
+  <si>
+    <t>[[1,10],[2,100]]</t>
+  </si>
+  <si>
+    <t>nested array</t>
+  </si>
+  <si>
+    <t>int16 array with uncertain length</t>
+  </si>
+  <si>
+    <t>integer array with specify length</t>
+  </si>
+  <si>
+    <t>json type. Start with '{' and end with '}' pair with key : &lt;value type&gt;</t>
+  </si>
+  <si>
+    <t>very_complex_object</t>
+  </si>
+  <si>
+    <t>a very complex object type</t>
+  </si>
+  <si>
+    <t>{k:{str:string[]}}[]</t>
+  </si>
+  <si>
+    <t>[{"k":{"str":["123","234"]}},{"k":{"str":["abc"]}}]</t>
+  </si>
+  <si>
+    <t>lxjc;s;ldfkjasldfj,;asldfkjsdfakljasdf l;asj;f;a,</t>
+  </si>
+  <si>
+    <t>A023;_ASDLFKJLJ;,</t>
+  </si>
+  <si>
+    <t>[]</t>
   </si>
 </sst>
 </file>
@@ -261,8 +240,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -601,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -620,183 +602,158 @@
     <col min="9" max="9" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="37.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.85546875" customWidth="1"/>
+    <col min="13" max="13" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" t="s">
+        <v>39</v>
+      </c>
+      <c r="N2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" t="s">
+        <v>37</v>
+      </c>
+      <c r="M3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="45">
+      <c r="A4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" t="s">
-        <v>28</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="D4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="L2" t="s">
+      <c r="G4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="M2" t="s">
-        <v>36</v>
-      </c>
-      <c r="N2" t="s">
-        <v>39</v>
-      </c>
-      <c r="O2" t="s">
-        <v>40</v>
-      </c>
-      <c r="P2" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>44</v>
+      <c r="L4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" t="s">
-        <v>50</v>
-      </c>
-      <c r="I3" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" t="s">
-        <v>29</v>
-      </c>
-      <c r="K3" t="s">
-        <v>51</v>
-      </c>
-      <c r="L3" t="s">
-        <v>11</v>
-      </c>
-      <c r="M3" t="s">
-        <v>11</v>
-      </c>
-      <c r="N3" t="s">
-        <v>6</v>
-      </c>
-      <c r="O3" t="s">
-        <v>11</v>
-      </c>
-      <c r="P3" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" t="s">
-        <v>31</v>
-      </c>
-      <c r="I4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" t="s">
-        <v>26</v>
-      </c>
-      <c r="K4" t="s">
-        <v>34</v>
-      </c>
-      <c r="L4" t="s">
-        <v>37</v>
-      </c>
-      <c r="M4" t="s">
-        <v>38</v>
-      </c>
-      <c r="N4" t="s">
-        <v>41</v>
-      </c>
-      <c r="O4" t="s">
-        <v>42</v>
-      </c>
-      <c r="P4" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:14">
       <c r="A5">
         <v>1000001</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D5">
         <v>100000</v>
@@ -811,34 +768,65 @@
         <v>1.0001111110000001</v>
       </c>
       <c r="H5" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="I5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5" t="s">
         <v>25</v>
       </c>
-      <c r="J5" t="s">
-        <v>27</v>
-      </c>
-      <c r="K5" t="s">
+      <c r="M5" t="s">
+        <v>41</v>
+      </c>
+      <c r="N5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6">
+        <v>1000002</v>
+      </c>
+      <c r="C6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6">
+        <v>-100000</v>
+      </c>
+      <c r="E6">
+        <v>32767</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>33333333333</v>
+      </c>
+      <c r="J6" t="s">
         <v>52</v>
       </c>
-      <c r="L5">
-        <v>100</v>
-      </c>
-      <c r="M5">
-        <v>200</v>
-      </c>
-      <c r="N5" t="s">
-        <v>47</v>
-      </c>
-      <c r="O5">
-        <v>1000</v>
-      </c>
-      <c r="P5" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q5">
-        <v>1000</v>
+      <c r="K6" t="s">
+        <v>52</v>
+      </c>
+      <c r="M6" t="s">
+        <v>52</v>
+      </c>
+      <c r="N6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7">
+        <v>1000003</v>
+      </c>
+      <c r="C7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7">
+        <v>-32768</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1.type check bug fix(base type check is unprecise)
</commit_message>
<xml_diff>
--- a/test/excel/Example.xlsx
+++ b/test/excel/Example.xlsx
@@ -3,19 +3,20 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{025E7DE6-4628-413D-9A9F-55A38EFA90E2}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{CBB82F8B-D982-499B-BE04-51281E01AD8D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
   <si>
     <t>Example</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -94,10 +95,6 @@
   </si>
   <si>
     <t>type_object</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"key1":10100,"key2":[100,200]}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -198,6 +195,24 @@
   </si>
   <si>
     <t>[]</t>
+  </si>
+  <si>
+    <t>TestCase</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>*int</t>
+  </si>
+  <si>
+    <t>{"key1":10100,"key2":20100}</t>
+  </si>
+  <si>
+    <t>{"key1":10100,"key2":1.0000000001}</t>
   </si>
 </sst>
 </file>
@@ -585,8 +600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -612,7 +627,7 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -623,10 +638,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
@@ -650,16 +665,16 @@
         <v>17</v>
       </c>
       <c r="K2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -682,7 +697,7 @@
         <v>12</v>
       </c>
       <c r="H3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I3" t="s">
         <v>14</v>
@@ -691,58 +706,58 @@
         <v>18</v>
       </c>
       <c r="K3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="45">
       <c r="A4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="L4" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -750,7 +765,7 @@
         <v>1000001</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -768,7 +783,7 @@
         <v>1.0001111110000001</v>
       </c>
       <c r="H5" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="I5" t="s">
         <v>15</v>
@@ -777,13 +792,13 @@
         <v>16</v>
       </c>
       <c r="K5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -791,7 +806,7 @@
         <v>1000002</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D6">
         <v>-100000</v>
@@ -806,16 +821,16 @@
         <v>33333333333</v>
       </c>
       <c r="J6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -823,7 +838,7 @@
         <v>1000003</v>
       </c>
       <c r="C7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E7">
         <v>-32768</v>
@@ -834,4 +849,48 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6028141-B9C3-4193-8A13-A5B453D7BB89}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="B1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
1.add underline for yellow output 2.add 'json' type example 3.fix 'json' type check error
</commit_message>
<xml_diff>
--- a/test/excel/Example.xlsx
+++ b/test/excel/Example.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{CBB82F8B-D982-499B-BE04-51281E01AD8D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="62">
   <si>
     <t>Example</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -213,13 +212,27 @@
   </si>
   <si>
     <t>{"key1":10100,"key2":1.0000000001}</t>
+  </si>
+  <si>
+    <t>effectParam</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"Box":"ys_015"}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>json</t>
+  </si>
+  <si>
+    <t>["box", 1, "test"]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -232,6 +245,14 @@
       <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -262,7 +283,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -278,7 +299,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -353,23 +374,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -405,23 +409,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -597,11 +584,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -625,7 +612,7 @@
     <col min="17" max="17" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -633,7 +620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -676,8 +663,11 @@
       <c r="N2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="3" spans="1:14">
+      <c r="O2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -717,8 +707,11 @@
       <c r="N3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" ht="45">
+      <c r="O3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="45">
       <c r="A4" s="1" t="s">
         <v>28</v>
       </c>
@@ -759,8 +752,11 @@
       <c r="N4" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="5" spans="1:14">
+      <c r="O4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5">
         <v>1000001</v>
       </c>
@@ -800,8 +796,11 @@
       <c r="N5" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="6" spans="1:14">
+      <c r="O5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6">
         <v>1000002</v>
       </c>
@@ -833,7 +832,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:15">
       <c r="A7">
         <v>1000003</v>
       </c>
@@ -852,12 +851,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6028141-B9C3-4193-8A13-A5B453D7BB89}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>

</xml_diff>

<commit_message>
1.fix type `vector2` `vector3` join with `[]` check error. FIXME: 1.fix date type format
</commit_message>
<xml_diff>
--- a/test/excel/Example.xlsx
+++ b/test/excel/Example.xlsx
@@ -1,21 +1,87 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6A017078-74CA-4C17-B44C-7DFAC0A5F992}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+SkyUser:
+结束时间0表示无限制
+有对应应活动ID，必须填0</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+结束时间0表示无限制</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="73">
   <si>
     <t>Example</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -211,9 +277,6 @@
     <t>{"key1":10100,"key2":20100}</t>
   </si>
   <si>
-    <t>{"key1":10100,"key2":1.0000000001}</t>
-  </si>
-  <si>
     <t>effectParam</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -226,13 +289,57 @@
   </si>
   <si>
     <t>["box", 1, "test"]</t>
+  </si>
+  <si>
+    <t>单品限购</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SingleShop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>begintime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>endtime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>购买开始时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>购买截止时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vector2[3]</t>
+  </si>
+  <si>
+    <t>vector3[2]</t>
+  </si>
+  <si>
+    <t>[[1,1],[2,2],[3,3]]</t>
+  </si>
+  <si>
+    <t>[[1,1,1],[2,2,2]]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -255,16 +362,60 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -272,20 +423,52 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+  <cellStyles count="3">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规 10" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="常规 15" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -299,7 +482,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -374,6 +557,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -409,6 +609,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -584,11 +801,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -664,7 +881,7 @@
         <v>45</v>
       </c>
       <c r="O2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -708,7 +925,7 @@
         <v>47</v>
       </c>
       <c r="O3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="45">
@@ -753,7 +970,7 @@
         <v>46</v>
       </c>
       <c r="O4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -797,7 +1014,7 @@
         <v>48</v>
       </c>
       <c r="O5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -851,19 +1068,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="B1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>53</v>
       </c>
@@ -871,23 +1090,382 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>69</v>
+      </c>
+      <c r="C3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>71</v>
+      </c>
+      <c r="C4" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:C30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="25.140625" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="3">
+        <v>1</v>
+      </c>
+      <c r="B5" s="4">
+        <v>43066.461574074077</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="3">
+        <v>2</v>
+      </c>
+      <c r="B6" s="4">
+        <v>43066.461574074077</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="3">
+        <v>3</v>
+      </c>
+      <c r="B7" s="4">
+        <v>43066.461574074077</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="3">
+        <v>4</v>
+      </c>
+      <c r="B8" s="4">
+        <v>43267.000011574077</v>
+      </c>
+      <c r="C8" s="4">
+        <v>43269.99931712963</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="3">
+        <v>5</v>
+      </c>
+      <c r="B9" s="4">
+        <v>43267.000011574077</v>
+      </c>
+      <c r="C9" s="4">
+        <v>43269.99931712963</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="3">
+        <v>78</v>
+      </c>
+      <c r="B10" s="4">
+        <v>43066.461574074077</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="3">
+        <v>79</v>
+      </c>
+      <c r="B11" s="4">
+        <v>43066.461574074077</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="3">
+        <v>80</v>
+      </c>
+      <c r="B12" s="4">
+        <v>43066.461574074077</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="3">
+        <v>81</v>
+      </c>
+      <c r="B13" s="4">
+        <v>43066.461574074077</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="3">
+        <v>82</v>
+      </c>
+      <c r="B14" s="4">
+        <v>43066.461574074077</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="3">
+        <v>83</v>
+      </c>
+      <c r="B15" s="4">
+        <v>43066.461574074077</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="3">
+        <v>84</v>
+      </c>
+      <c r="B16" s="4">
+        <v>43066.461574074077</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="3">
+        <v>85</v>
+      </c>
+      <c r="B17" s="4">
+        <v>43066.461574074077</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="3">
+        <v>86</v>
+      </c>
+      <c r="B18" s="4">
+        <v>43066.461574074077</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="3">
+        <v>87</v>
+      </c>
+      <c r="B19" s="4">
+        <v>43066.461574074077</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="3">
+        <v>88</v>
+      </c>
+      <c r="B20" s="4">
+        <v>43066.461574074077</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="3">
+        <v>89</v>
+      </c>
+      <c r="B21" s="4">
+        <v>43066.461574074077</v>
+      </c>
+      <c r="C21" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="3">
+        <v>90</v>
+      </c>
+      <c r="B22" s="4">
+        <v>43066.461574074077</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="3">
+        <v>91</v>
+      </c>
+      <c r="B23" s="4">
+        <v>43066.461574074077</v>
+      </c>
+      <c r="C23" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="3">
+        <v>92</v>
+      </c>
+      <c r="B24" s="4">
+        <v>43066.461574074077</v>
+      </c>
+      <c r="C24" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="3">
+        <v>93</v>
+      </c>
+      <c r="B25" s="4">
+        <v>43066.461574074077</v>
+      </c>
+      <c r="C25" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="3">
+        <v>94</v>
+      </c>
+      <c r="B26" s="4">
+        <v>43066.461574074077</v>
+      </c>
+      <c r="C26" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="3">
+        <v>95</v>
+      </c>
+      <c r="B27" s="4">
+        <v>43066.461574074077</v>
+      </c>
+      <c r="C27" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="3">
+        <v>96</v>
+      </c>
+      <c r="B28" s="4">
+        <v>43066.461574074077</v>
+      </c>
+      <c r="C28" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="3">
+        <v>97</v>
+      </c>
+      <c r="B29" s="4">
+        <v>43066.461574074077</v>
+      </c>
+      <c r="C29" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="3">
+        <v>98</v>
+      </c>
+      <c r="B30" s="4">
+        <v>43066.461574074077</v>
+      </c>
+      <c r="C30" s="3">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:C4 C5:C7 A2:A30 C10:C30">
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>IF(COUNTIF($2:$2,A$2)&gt;1,1,0)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
1.support date types export.
******
FIXME:
1.utctime is incorrect
</commit_message>
<xml_diff>
--- a/test/excel/Example.xlsx
+++ b/test/excel/Example.xlsx
@@ -3,85 +3,20 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6A017078-74CA-4C17-B44C-7DFAC0A5F992}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{596D1761-EE30-431D-9C13-AD7DC78CA150}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Author</author>
-  </authors>
-  <commentList>
-    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">
-SkyUser:
-结束时间0表示无限制
-有对应应活动ID，必须填0</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">
-结束时间0表示无限制</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="73">
   <si>
     <t>Example</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -291,38 +226,6 @@
     <t>["box", 1, "test"]</t>
   </si>
   <si>
-    <t>单品限购</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SingleShop</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>begintime</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>endtime</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>#ID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>购买开始时间</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>购买截止时间</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>vector2[3]</t>
   </si>
   <si>
@@ -333,13 +236,37 @@
   </si>
   <si>
     <t>[[1,1,1],[2,2,2]]</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>tinydate</t>
+  </si>
+  <si>
+    <t>timestamp</t>
+  </si>
+  <si>
+    <t>utctime</t>
+  </si>
+  <si>
+    <t>encode with DateFMT</t>
+  </si>
+  <si>
+    <t>encode with TinyDateFMT</t>
+  </si>
+  <si>
+    <t>linux time stamp</t>
+  </si>
+  <si>
+    <t>utc time stamp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -363,15 +290,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -379,43 +297,16 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -423,52 +314,25 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="0"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="常规 10" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="常规 15" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -802,10 +666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -827,9 +691,10 @@
     <col min="15" max="15" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:19">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -837,7 +702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:19">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -883,8 +748,20 @@
       <c r="O2" t="s">
         <v>57</v>
       </c>
+      <c r="P2" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>66</v>
+      </c>
+      <c r="R2" t="s">
+        <v>67</v>
+      </c>
+      <c r="S2" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:19">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -927,8 +804,20 @@
       <c r="O3" t="s">
         <v>59</v>
       </c>
+      <c r="P3" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>66</v>
+      </c>
+      <c r="R3" t="s">
+        <v>67</v>
+      </c>
+      <c r="S3" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="4" spans="1:15" ht="45">
+    <row r="4" spans="1:19" ht="45">
       <c r="A4" s="1" t="s">
         <v>28</v>
       </c>
@@ -972,8 +861,20 @@
       <c r="O4" t="s">
         <v>60</v>
       </c>
+      <c r="P4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>72</v>
+      </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:19">
       <c r="A5">
         <v>1000001</v>
       </c>
@@ -1016,8 +917,20 @@
       <c r="O5" t="s">
         <v>58</v>
       </c>
+      <c r="P5" s="2">
+        <v>43415</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>43415</v>
+      </c>
+      <c r="R5" s="2">
+        <v>43415</v>
+      </c>
+      <c r="S5" s="2">
+        <v>43415</v>
+      </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:19">
       <c r="A6">
         <v>1000002</v>
       </c>
@@ -1048,8 +961,20 @@
       <c r="N6" t="s">
         <v>51</v>
       </c>
+      <c r="P6" s="2">
+        <v>43831.499988425923</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>43831.499988425923</v>
+      </c>
+      <c r="R6" s="2">
+        <v>43831.499988425923</v>
+      </c>
+      <c r="S6" s="2">
+        <v>43831.499988425923</v>
+      </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:19">
       <c r="A7">
         <v>1000003</v>
       </c>
@@ -1071,8 +996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1095,10 +1020,10 @@
         <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1106,366 +1031,13 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C4" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C30"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="25.140625" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C1" s="3"/>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="3">
-        <v>1</v>
-      </c>
-      <c r="B5" s="4">
-        <v>43066.461574074077</v>
-      </c>
-      <c r="C5" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="3">
-        <v>2</v>
-      </c>
-      <c r="B6" s="4">
-        <v>43066.461574074077</v>
-      </c>
-      <c r="C6" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="3">
-        <v>3</v>
-      </c>
-      <c r="B7" s="4">
-        <v>43066.461574074077</v>
-      </c>
-      <c r="C7" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="3">
-        <v>4</v>
-      </c>
-      <c r="B8" s="4">
-        <v>43267.000011574077</v>
-      </c>
-      <c r="C8" s="4">
-        <v>43269.99931712963</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="3">
-        <v>5</v>
-      </c>
-      <c r="B9" s="4">
-        <v>43267.000011574077</v>
-      </c>
-      <c r="C9" s="4">
-        <v>43269.99931712963</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="3">
-        <v>78</v>
-      </c>
-      <c r="B10" s="4">
-        <v>43066.461574074077</v>
-      </c>
-      <c r="C10" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="3">
-        <v>79</v>
-      </c>
-      <c r="B11" s="4">
-        <v>43066.461574074077</v>
-      </c>
-      <c r="C11" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="3">
-        <v>80</v>
-      </c>
-      <c r="B12" s="4">
-        <v>43066.461574074077</v>
-      </c>
-      <c r="C12" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="3">
-        <v>81</v>
-      </c>
-      <c r="B13" s="4">
-        <v>43066.461574074077</v>
-      </c>
-      <c r="C13" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="3">
-        <v>82</v>
-      </c>
-      <c r="B14" s="4">
-        <v>43066.461574074077</v>
-      </c>
-      <c r="C14" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="3">
-        <v>83</v>
-      </c>
-      <c r="B15" s="4">
-        <v>43066.461574074077</v>
-      </c>
-      <c r="C15" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="3">
-        <v>84</v>
-      </c>
-      <c r="B16" s="4">
-        <v>43066.461574074077</v>
-      </c>
-      <c r="C16" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="3">
-        <v>85</v>
-      </c>
-      <c r="B17" s="4">
-        <v>43066.461574074077</v>
-      </c>
-      <c r="C17" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="3">
-        <v>86</v>
-      </c>
-      <c r="B18" s="4">
-        <v>43066.461574074077</v>
-      </c>
-      <c r="C18" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="3">
-        <v>87</v>
-      </c>
-      <c r="B19" s="4">
-        <v>43066.461574074077</v>
-      </c>
-      <c r="C19" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="3">
-        <v>88</v>
-      </c>
-      <c r="B20" s="4">
-        <v>43066.461574074077</v>
-      </c>
-      <c r="C20" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="3">
-        <v>89</v>
-      </c>
-      <c r="B21" s="4">
-        <v>43066.461574074077</v>
-      </c>
-      <c r="C21" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="3">
-        <v>90</v>
-      </c>
-      <c r="B22" s="4">
-        <v>43066.461574074077</v>
-      </c>
-      <c r="C22" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="3">
-        <v>91</v>
-      </c>
-      <c r="B23" s="4">
-        <v>43066.461574074077</v>
-      </c>
-      <c r="C23" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="3">
-        <v>92</v>
-      </c>
-      <c r="B24" s="4">
-        <v>43066.461574074077</v>
-      </c>
-      <c r="C24" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="3">
-        <v>93</v>
-      </c>
-      <c r="B25" s="4">
-        <v>43066.461574074077</v>
-      </c>
-      <c r="C25" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="3">
-        <v>94</v>
-      </c>
-      <c r="B26" s="4">
-        <v>43066.461574074077</v>
-      </c>
-      <c r="C26" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="3">
-        <v>95</v>
-      </c>
-      <c r="B27" s="4">
-        <v>43066.461574074077</v>
-      </c>
-      <c r="C27" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="3">
-        <v>96</v>
-      </c>
-      <c r="B28" s="4">
-        <v>43066.461574074077</v>
-      </c>
-      <c r="C28" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="3">
-        <v>97</v>
-      </c>
-      <c r="B29" s="4">
-        <v>43066.461574074077</v>
-      </c>
-      <c r="C29" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="3">
-        <v>98</v>
-      </c>
-      <c r="B30" s="4">
-        <v>43066.461574074077</v>
-      </c>
-      <c r="C30" s="3">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="B2:C4 C5:C7 A2:A30 C10:C30">
-    <cfRule type="expression" dxfId="0" priority="2">
-      <formula>IF(COUNTIF($2:$2,A$2)&gt;1,1,0)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
1.fix date type check error 2.complete async mode 3.add date type test case
******
FIXME:
1.complete `README.md`
2.fix integer has decimal point error
</commit_message>
<xml_diff>
--- a/test/excel/Example.xlsx
+++ b/test/excel/Example.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{596D1761-EE30-431D-9C13-AD7DC78CA150}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="84">
   <si>
     <t>Example</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -260,12 +259,45 @@
   </si>
   <si>
     <t>utc time stamp</t>
+  </si>
+  <si>
+    <t>{k:date}</t>
+  </si>
+  <si>
+    <t>dateArry</t>
+  </si>
+  <si>
+    <t>date in object value</t>
+  </si>
+  <si>
+    <t>date array</t>
+  </si>
+  <si>
+    <t>["2018/01/01 23:59:59"]</t>
+  </si>
+  <si>
+    <t>date[1]</t>
+  </si>
+  <si>
+    <t>timestamparry</t>
+  </si>
+  <si>
+    <t>timestamp[2]</t>
+  </si>
+  <si>
+    <t>timestamp array</t>
+  </si>
+  <si>
+    <t>[1529995094, 1529995116]</t>
+  </si>
+  <si>
+    <t>{"k":"2018/01/01 00:59:59"}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -328,9 +360,9 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="常规 10" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="常规 15" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="常规 10" xfId="1"/>
+    <cellStyle name="常规 15" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -346,7 +378,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -421,23 +453,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -473,23 +488,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -665,11 +663,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="W5" sqref="W5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -692,9 +690,12 @@
     <col min="16" max="16" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="26.85546875" customWidth="1"/>
+    <col min="21" max="21" width="17.28515625" customWidth="1"/>
+    <col min="22" max="22" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:22">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -702,7 +703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:22">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -760,8 +761,17 @@
       <c r="S2" t="s">
         <v>68</v>
       </c>
+      <c r="T2" t="s">
+        <v>65</v>
+      </c>
+      <c r="U2" t="s">
+        <v>74</v>
+      </c>
+      <c r="V2" t="s">
+        <v>79</v>
+      </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:22">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -816,8 +826,17 @@
       <c r="S3" t="s">
         <v>68</v>
       </c>
+      <c r="T3" t="s">
+        <v>73</v>
+      </c>
+      <c r="U3" t="s">
+        <v>78</v>
+      </c>
+      <c r="V3" t="s">
+        <v>80</v>
+      </c>
     </row>
-    <row r="4" spans="1:19" ht="45">
+    <row r="4" spans="1:22" ht="45">
       <c r="A4" s="1" t="s">
         <v>28</v>
       </c>
@@ -873,8 +892,17 @@
       <c r="S4" s="1" t="s">
         <v>72</v>
       </c>
+      <c r="T4" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:22">
       <c r="A5">
         <v>1000001</v>
       </c>
@@ -929,8 +957,17 @@
       <c r="S5" s="2">
         <v>43415</v>
       </c>
+      <c r="T5" t="s">
+        <v>83</v>
+      </c>
+      <c r="U5" t="s">
+        <v>77</v>
+      </c>
+      <c r="V5" t="s">
+        <v>82</v>
+      </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:22">
       <c r="A6">
         <v>1000002</v>
       </c>
@@ -974,7 +1011,7 @@
         <v>43831.499988425923</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:22">
       <c r="A7">
         <v>1000003</v>
       </c>
@@ -993,7 +1030,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
1.fix integer has decimal point error 2.remove module `exceljs` 3.complete date type check and value exchange 4.fix time config bug 5.add fraction digits configure 6.add test case for double and float
******
FIXME:
1.complete `README.md`
</commit_message>
<xml_diff>
--- a/test/excel/Example.xlsx
+++ b/test/excel/Example.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="86">
   <si>
     <t>Example</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -160,9 +160,6 @@
     <t>int[][2]</t>
   </si>
   <si>
-    <t>[[1,10],[2,100]]</t>
-  </si>
-  <si>
     <t>nested array</t>
   </si>
   <si>
@@ -292,6 +289,15 @@
   </si>
   <si>
     <t>{"k":"2018/01/01 00:59:59"}</t>
+  </si>
+  <si>
+    <t>double</t>
+  </si>
+  <si>
+    <t>[[1,10],[2,100.10]]</t>
+  </si>
+  <si>
+    <t>double clip</t>
   </si>
 </sst>
 </file>
@@ -664,10 +670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V7"/>
+  <dimension ref="A1:W7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="W5" sqref="W5"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="W8" sqref="W8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -693,9 +699,10 @@
     <col min="20" max="20" width="26.85546875" customWidth="1"/>
     <col min="21" max="21" width="17.28515625" customWidth="1"/>
     <col min="22" max="22" width="18.28515625" customWidth="1"/>
+    <col min="23" max="23" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:23">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -703,7 +710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:23">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -744,34 +751,37 @@
         <v>38</v>
       </c>
       <c r="N2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P2" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q2" t="s">
         <v>65</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>66</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>67</v>
       </c>
-      <c r="S2" t="s">
-        <v>68</v>
-      </c>
       <c r="T2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="U2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="V2" t="s">
-        <v>79</v>
+        <v>78</v>
+      </c>
+      <c r="W2" t="s">
+        <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:23">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -809,34 +819,37 @@
         <v>39</v>
       </c>
       <c r="N3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P3" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q3" t="s">
         <v>65</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>66</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>67</v>
       </c>
-      <c r="S3" t="s">
-        <v>68</v>
-      </c>
       <c r="T3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="U3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="V3" t="s">
-        <v>80</v>
+        <v>79</v>
+      </c>
+      <c r="W3" t="s">
+        <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="45">
+    <row r="4" spans="1:23" ht="45">
       <c r="A4" s="1" t="s">
         <v>28</v>
       </c>
@@ -857,13 +870,13 @@
         <v>33</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>34</v>
@@ -872,37 +885,40 @@
         <v>37</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q4" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="R4" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="R4" s="1" t="s">
+      <c r="S4" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="S4" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="T4" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="U4" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="U4" s="1" t="s">
-        <v>76</v>
-      </c>
       <c r="V4" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:23">
       <c r="A5">
         <v>1000001</v>
       </c>
@@ -925,7 +941,7 @@
         <v>1.0001111110000001</v>
       </c>
       <c r="H5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I5" t="s">
         <v>15</v>
@@ -937,13 +953,13 @@
         <v>24</v>
       </c>
       <c r="M5" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="N5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="P5" s="2">
         <v>43415</v>
@@ -958,21 +974,24 @@
         <v>43415</v>
       </c>
       <c r="T5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="U5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="V5" t="s">
-        <v>82</v>
+        <v>81</v>
+      </c>
+      <c r="W5">
+        <v>1123.0123456788999</v>
       </c>
     </row>
-    <row r="6" spans="1:22">
+    <row r="6" spans="1:23">
       <c r="A6">
         <v>1000002</v>
       </c>
       <c r="C6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D6">
         <v>-100000</v>
@@ -987,16 +1006,16 @@
         <v>33333333333</v>
       </c>
       <c r="J6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P6" s="2">
         <v>43831.499988425923</v>
@@ -1010,16 +1029,22 @@
       <c r="S6" s="2">
         <v>43831.499988425923</v>
       </c>
+      <c r="W6">
+        <v>1.555555555</v>
+      </c>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:23">
       <c r="A7">
         <v>1000003</v>
       </c>
       <c r="C7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E7">
         <v>-32768</v>
+      </c>
+      <c r="W7">
+        <v>0.230000123</v>
       </c>
     </row>
   </sheetData>
@@ -1041,26 +1066,26 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="B1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" t="s">
         <v>53</v>
-      </c>
-      <c r="B2" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" t="s">
         <v>61</v>
-      </c>
-      <c r="C3" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1068,10 +1093,10 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" t="s">
         <v>63</v>
-      </c>
-      <c r="C4" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1.add json value type fixed 2.add test case
******
FIXME:
1.complete README.md
</commit_message>
<xml_diff>
--- a/test/excel/Example.xlsx
+++ b/test/excel/Example.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D6B66002-293B-4215-8431-F1EFFA84A092}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="91">
   <si>
     <t>Example</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -199,9 +200,6 @@
     <t>id</t>
   </si>
   <si>
-    <t>type</t>
-  </si>
-  <si>
     <t>*int</t>
   </si>
   <si>
@@ -298,12 +296,30 @@
   </si>
   <si>
     <t>double clip</t>
+  </si>
+  <si>
+    <t>name1</t>
+  </si>
+  <si>
+    <t>name2</t>
+  </si>
+  <si>
+    <t>[[1.0,0.1],[1,1],[2,2]]</t>
+  </si>
+  <si>
+    <t>timestamp_arry</t>
+  </si>
+  <si>
+    <t>timestamp[]</t>
+  </si>
+  <si>
+    <t>["2018/12/31 00:00:00"]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -366,9 +382,9 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="常规 10" xfId="1"/>
-    <cellStyle name="常规 15" xfId="2"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规 10" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="常规 15" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -384,7 +400,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -459,6 +475,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -494,6 +527,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -669,11 +719,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="W8" sqref="W8"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="W9" sqref="W9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -754,31 +804,31 @@
         <v>44</v>
       </c>
       <c r="O2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="P2" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q2" t="s">
         <v>64</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>65</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>66</v>
       </c>
-      <c r="S2" t="s">
-        <v>67</v>
-      </c>
       <c r="T2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="U2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="V2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="W2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:23">
@@ -822,31 +872,31 @@
         <v>46</v>
       </c>
       <c r="O3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="P3" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q3" t="s">
         <v>64</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>65</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>66</v>
       </c>
-      <c r="S3" t="s">
-        <v>67</v>
-      </c>
       <c r="T3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="U3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="V3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="W3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="45">
@@ -891,31 +941,31 @@
         <v>45</v>
       </c>
       <c r="O4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q4" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="R4" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="R4" s="1" t="s">
+      <c r="S4" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="S4" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="T4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="U4" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="U4" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="V4" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="W4" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:23">
@@ -941,7 +991,7 @@
         <v>1.0001111110000001</v>
       </c>
       <c r="H5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I5" t="s">
         <v>15</v>
@@ -953,13 +1003,13 @@
         <v>24</v>
       </c>
       <c r="M5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="N5" t="s">
         <v>47</v>
       </c>
       <c r="O5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P5" s="2">
         <v>43415</v>
@@ -974,13 +1024,13 @@
         <v>43415</v>
       </c>
       <c r="T5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="U5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="V5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="W5">
         <v>1123.0123456788999</v>
@@ -1055,48 +1105,71 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="B1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>52</v>
       </c>
       <c r="B2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
         <v>53</v>
       </c>
+      <c r="B3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" t="s">
+        <v>89</v>
+      </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" t="s">
         <v>62</v>
       </c>
-      <c r="C4" t="s">
-        <v>63</v>
+      <c r="D4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1.add load configure file from `process.argv` and check types. 2.Code optimization
</commit_message>
<xml_diff>
--- a/test/excel/Example.xlsx
+++ b/test/excel/Example.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D6B66002-293B-4215-8431-F1EFFA84A092}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -283,9 +282,6 @@
     <t>timestamp array</t>
   </si>
   <si>
-    <t>[1529995094, 1529995116]</t>
-  </si>
-  <si>
     <t>{"k":"2018/01/01 00:59:59"}</t>
   </si>
   <si>
@@ -314,12 +310,15 @@
   </si>
   <si>
     <t>["2018/12/31 00:00:00"]</t>
+  </si>
+  <si>
+    <t>["2018/01/01 00:00:00", "2018/01/01 23:59:59"]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -382,9 +381,9 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="常规 10" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="常规 15" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="常规 10" xfId="1"/>
+    <cellStyle name="常规 15" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -400,7 +399,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -475,23 +474,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -527,23 +509,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -719,11 +684,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W7"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="W9" sqref="W9"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="V6" sqref="V6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -828,7 +793,7 @@
         <v>77</v>
       </c>
       <c r="W2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:23">
@@ -896,7 +861,7 @@
         <v>78</v>
       </c>
       <c r="W3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="45">
@@ -965,7 +930,7 @@
         <v>79</v>
       </c>
       <c r="W4" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:23">
@@ -1003,7 +968,7 @@
         <v>24</v>
       </c>
       <c r="M5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N5" t="s">
         <v>47</v>
@@ -1024,13 +989,13 @@
         <v>43415</v>
       </c>
       <c r="T5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="U5" t="s">
         <v>75</v>
       </c>
       <c r="V5" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="W5">
         <v>1123.0123456788999</v>
@@ -1105,11 +1070,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1124,13 +1089,13 @@
         <v>52</v>
       </c>
       <c r="B2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" t="s">
         <v>85</v>
       </c>
-      <c r="C2" t="s">
-        <v>86</v>
-      </c>
       <c r="D2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1144,7 +1109,7 @@
         <v>60</v>
       </c>
       <c r="D3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1166,10 +1131,10 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1.add js "'" translate to "\'"
</commit_message>
<xml_diff>
--- a/test/excel/Example.xlsx
+++ b/test/excel/Example.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C136ED27-7FA5-4729-88C1-DC071C97F26C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{64E3E54C-F6E7-433A-B384-9469DDD9C41D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,10 +35,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>xxxx</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>type_int</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -330,6 +326,9 @@
   </si>
   <si>
     <t>bool</t>
+  </si>
+  <si>
+    <t>123'456'zzz</t>
   </si>
 </sst>
 </file>
@@ -390,12 +389,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -738,8 +738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W7"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="V6" sqref="V6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -770,7 +770,7 @@
   <sheetData>
     <row r="1" spans="1:23">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -781,70 +781,70 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" t="s">
         <v>19</v>
       </c>
-      <c r="I2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" t="s">
-        <v>20</v>
-      </c>
       <c r="L2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="P2" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q2" t="s">
         <v>63</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>64</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>65</v>
       </c>
-      <c r="S2" t="s">
-        <v>66</v>
-      </c>
       <c r="T2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="U2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="V2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="W2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:23">
@@ -855,133 +855,133 @@
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" t="s">
         <v>22</v>
       </c>
-      <c r="I3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K3" t="s">
-        <v>23</v>
-      </c>
       <c r="L3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P3" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q3" t="s">
         <v>63</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>64</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>65</v>
       </c>
-      <c r="S3" t="s">
-        <v>66</v>
-      </c>
       <c r="T3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="U3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="V3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="W3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="45">
       <c r="A4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="L4" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="P4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q4" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="R4" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="R4" s="1" t="s">
+      <c r="S4" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="S4" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="T4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="U4" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="U4" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="V4" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="W4" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:23">
@@ -989,10 +989,10 @@
         <v>1000001</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
+        <v>26</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="D5">
         <v>100000</v>
@@ -1007,25 +1007,25 @@
         <v>1.0001111110000001</v>
       </c>
       <c r="H5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" t="s">
         <v>15</v>
       </c>
-      <c r="J5" t="s">
-        <v>16</v>
-      </c>
       <c r="K5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="P5" s="2">
         <v>43415</v>
@@ -1040,13 +1040,13 @@
         <v>43415</v>
       </c>
       <c r="T5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="U5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="V5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="W5">
         <v>1123.0123456788999</v>
@@ -1057,7 +1057,7 @@
         <v>1000002</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D6">
         <v>-100000</v>
@@ -1072,16 +1072,16 @@
         <v>33333333333</v>
       </c>
       <c r="J6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="P6" s="2">
         <v>43831.499988425923</v>
@@ -1104,7 +1104,7 @@
         <v>1000003</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E7">
         <v>-32768</v>
@@ -1132,35 +1132,35 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" t="s">
         <v>84</v>
       </c>
-      <c r="C2" t="s">
-        <v>85</v>
-      </c>
       <c r="D2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" t="s">
         <v>59</v>
       </c>
-      <c r="C3" t="s">
-        <v>60</v>
-      </c>
       <c r="D3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1168,13 +1168,13 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" t="s">
         <v>61</v>
       </c>
-      <c r="C4" t="s">
-        <v>62</v>
-      </c>
       <c r="D4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1182,10 +1182,10 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1197,34 +1197,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14D5ACE0-0A26-44C1-A471-1A8E141FFD6F}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" t="s">
         <v>94</v>
-      </c>
-      <c r="B3" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:2">

</xml_diff>

<commit_message>
remove multi line string support for some unresolved bugs
</commit_message>
<xml_diff>
--- a/test/excel/Example.xlsx
+++ b/test/excel/Example.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="98">
   <si>
     <t>{B1}is csv file name</t>
   </si>
@@ -93,7 +93,7 @@
     <t>double</t>
   </si>
   <si>
-    <t>string2</t>
+    <t>#string2</t>
   </si>
   <si>
     <t>*int</t>
@@ -212,6 +212,10 @@
   </si>
   <si>
     <t>double clip</t>
+  </si>
+  <si>
+    <t>temporary not support
+need to fix bugs...</t>
   </si>
   <si>
     <t>desc etc…</t>
@@ -927,12 +931,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="51">
@@ -1287,7 +1294,7 @@
   <dimension ref="A1:X28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="X6" sqref="X6"/>
+      <selection activeCell="X5" sqref="X5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1470,7 +1477,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" ht="40.5" spans="1:23">
+    <row r="4" ht="54" spans="1:24">
       <c r="A4" s="1" t="s">
         <v>43</v>
       </c>
@@ -1538,16 +1545,19 @@
       <c r="W4" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="X4" s="3" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="5" ht="67.5" spans="1:24">
       <c r="A5">
         <v>1000001</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C5" s="3" t="s">
         <v>66</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="D5">
         <v>100000</v>
@@ -1562,25 +1572,25 @@
         <v>1.000111111</v>
       </c>
       <c r="H5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="K5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="M5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="N5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="O5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="P5" s="2">
         <v>43415</v>
@@ -1595,19 +1605,19 @@
         <v>43415</v>
       </c>
       <c r="T5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="U5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="V5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="W5">
         <v>1123.0123456789</v>
       </c>
       <c r="X5" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:23">
@@ -1615,7 +1625,7 @@
         <v>1000002</v>
       </c>
       <c r="C6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D6">
         <v>-100000</v>
@@ -1630,16 +1640,16 @@
         <v>33333333333</v>
       </c>
       <c r="J6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="M6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="N6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="P6" s="2">
         <v>43831.4999884259</v>
@@ -1662,7 +1672,7 @@
         <v>1000003</v>
       </c>
       <c r="C7" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E7">
         <v>-32768</v>
@@ -1697,7 +1707,7 @@
   <sheetData>
     <row r="1" spans="2:2">
       <c r="B1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1705,13 +1715,13 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1719,13 +1729,13 @@
         <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1733,13 +1743,13 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1747,10 +1757,10 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1772,10 +1782,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1783,15 +1793,15 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:2">

</xml_diff>

<commit_message>
add color filter test
</commit_message>
<xml_diff>
--- a/test/excel/Example.xlsx
+++ b/test/excel/Example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12615"/>
+    <workbookView windowWidth="24345" windowHeight="12615" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -324,9 +324,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -337,10 +337,102 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -353,45 +445,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -413,37 +467,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -457,31 +480,8 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -490,43 +490,193 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -538,139 +688,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -684,11 +702,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -708,21 +732,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -734,11 +743,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -767,17 +791,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -787,10 +805,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -799,147 +817,147 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="51">
@@ -1293,8 +1311,8 @@
   <sheetPr/>
   <dimension ref="A1:X28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="X5" sqref="X5"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1339,34 +1357,34 @@
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="M2" t="s">
@@ -1478,74 +1496,74 @@
       </c>
     </row>
     <row r="4" ht="54" spans="1:24">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="4"/>
+      <c r="C4" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="K4" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="L4" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="M4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="N4" s="4" t="s">
         <v>55</v>
       </c>
       <c r="O4" t="s">
         <v>56</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="P4" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="Q4" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="R4" s="1" t="s">
+      <c r="R4" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="S4" s="1" t="s">
+      <c r="S4" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="T4" s="1" t="s">
+      <c r="T4" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="U4" s="1" t="s">
+      <c r="U4" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="V4" s="1" t="s">
+      <c r="V4" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="W4" s="1" t="s">
+      <c r="W4" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="X4" s="3" t="s">
+      <c r="X4" s="4" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1556,7 +1574,7 @@
       <c r="B5" t="s">
         <v>66</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="6" t="s">
         <v>67</v>
       </c>
       <c r="D5">
@@ -1592,16 +1610,16 @@
       <c r="O5" t="s">
         <v>74</v>
       </c>
-      <c r="P5" s="2">
+      <c r="P5" s="5">
         <v>43415</v>
       </c>
-      <c r="Q5" s="2">
+      <c r="Q5" s="5">
         <v>43415</v>
       </c>
-      <c r="R5" s="2">
+      <c r="R5" s="5">
         <v>43415</v>
       </c>
-      <c r="S5" s="2">
+      <c r="S5" s="5">
         <v>43415</v>
       </c>
       <c r="T5" t="s">
@@ -1616,7 +1634,7 @@
       <c r="W5">
         <v>1123.0123456789</v>
       </c>
-      <c r="X5" s="1" t="s">
+      <c r="X5" s="4" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1651,16 +1669,16 @@
       <c r="N6" t="s">
         <v>80</v>
       </c>
-      <c r="P6" s="2">
+      <c r="P6" s="5">
         <v>43831.4999884259</v>
       </c>
-      <c r="Q6" s="2">
+      <c r="Q6" s="5">
         <v>43831.4999884259</v>
       </c>
-      <c r="R6" s="2">
+      <c r="R6" s="5">
         <v>43831.4999884259</v>
       </c>
-      <c r="S6" s="2">
+      <c r="S6" s="5">
         <v>43831.4999884259</v>
       </c>
       <c r="W6">
@@ -1682,10 +1700,10 @@
       </c>
     </row>
     <row r="27" spans="19:19">
-      <c r="S27" s="1"/>
+      <c r="S27" s="4"/>
     </row>
     <row r="28" spans="20:20">
-      <c r="T28" s="1"/>
+      <c r="T28" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1699,8 +1717,8 @@
   <sheetPr/>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="3"/>
@@ -1714,13 +1732,13 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>85</v>
       </c>
     </row>

</xml_diff>